<commit_message>
e3 bug fixed; and result
</commit_message>
<xml_diff>
--- a/result/E3.xlsx
+++ b/result/E3.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhaos\Desktop\research-dual-period\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F78C50-6EFD-4A99-B94B-A5CA136F8318}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA65EF6-1194-42FF-8FB7-DD4CC709A8F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C7D420CA-42D4-4E62-9CB7-56532C9F3227}"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="11" r:id="rId1"/>
-    <sheet name="0.10" sheetId="5" r:id="rId2"/>
-    <sheet name="0.13" sheetId="4" r:id="rId3"/>
-    <sheet name="0.16" sheetId="3" r:id="rId4"/>
-    <sheet name="0.19" sheetId="2" r:id="rId5"/>
-    <sheet name="0.22" sheetId="1" r:id="rId6"/>
-    <sheet name="0.25" sheetId="6" r:id="rId7"/>
-    <sheet name="0.28" sheetId="7" r:id="rId8"/>
-    <sheet name="0.31" sheetId="8" r:id="rId9"/>
-    <sheet name="0.34" sheetId="9" r:id="rId10"/>
-    <sheet name="0.37" sheetId="10" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
+    <sheet name="summary" sheetId="11" r:id="rId2"/>
+    <sheet name="0.10" sheetId="5" r:id="rId3"/>
+    <sheet name="0.13" sheetId="4" r:id="rId4"/>
+    <sheet name="0.16" sheetId="3" r:id="rId5"/>
+    <sheet name="0.19" sheetId="2" r:id="rId6"/>
+    <sheet name="0.22" sheetId="1" r:id="rId7"/>
+    <sheet name="0.25" sheetId="6" r:id="rId8"/>
+    <sheet name="0.28" sheetId="7" r:id="rId9"/>
+    <sheet name="0.31" sheetId="8" r:id="rId10"/>
+    <sheet name="0.34" sheetId="9" r:id="rId11"/>
+    <sheet name="0.37" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="42">
   <si>
     <t>Best</t>
   </si>
@@ -100,6 +101,86 @@
     <t>solution</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SINGLE:</t>
+  </si>
+  <si>
+    <t>Util:0.10</t>
+  </si>
+  <si>
+    <t>Takset</t>
+  </si>
+  <si>
+    <t>#:</t>
+  </si>
+  <si>
+    <t>Fitable</t>
+  </si>
+  <si>
+    <t>tasks:</t>
+  </si>
+  <si>
+    <t>penalty</t>
+  </si>
+  <si>
+    <t>Util:0.13</t>
+  </si>
+  <si>
+    <t>Util:0.16</t>
+  </si>
+  <si>
+    <t>Util:0.19</t>
+  </si>
+  <si>
+    <t>\r\r</t>
+  </si>
+  <si>
+    <t>DUAL:</t>
+  </si>
+  <si>
+    <t>Util:0.22</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>single</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -144,9 +225,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,272 +551,3772 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE1F27B-438F-49BB-B1F9-9E2E3BFD9632}">
-  <dimension ref="A8:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE8625D-1816-4CE6-97F4-E7BD14C709EC}">
+  <dimension ref="A1:AH236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="P135" sqref="P135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>0.97</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>0.97</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4">
+        <f>MIN(J4:J13)</f>
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <f>MIN(K4:K13)</f>
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>0.996</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>0.996</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(J4:J13)</f>
+        <v>8.4</v>
+      </c>
+      <c r="O5">
+        <f>AVERAGE(K4:K13)</f>
+        <v>0.98580000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="M6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6">
+        <f>MAX(J4:J13)</f>
+        <v>11</v>
+      </c>
+      <c r="O6">
+        <f>MAX(K4:K13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>0.995</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>0.77139999999999997</v>
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>0.79630000000000001</v>
-      </c>
-      <c r="D8">
-        <v>0.79579999999999995</v>
-      </c>
-      <c r="E8">
-        <v>0.84899999999999998</v>
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
       </c>
       <c r="F8">
-        <f>0.6627+0.22</f>
-        <v>0.88269999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="M16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16">
+        <f>MIN(J16:J25)</f>
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <f>MIN(K16:K25)</f>
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17">
+        <v>0.995</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>0.995</v>
+      </c>
+      <c r="M17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17">
+        <f>AVERAGE(J16:J25)</f>
+        <v>7.3</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(K16:K25)</f>
+        <v>0.98629999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18">
+        <f>MAX(J16:J25)</f>
+        <v>10</v>
+      </c>
+      <c r="O18">
+        <f>MAX(K16:K25)</f>
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J20">
+        <v>7</v>
+      </c>
+      <c r="K20">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>0.99099999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+      <c r="K23">
+        <v>0.99099999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>0.997</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="M28" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28">
+        <f>MIN(J28:J37)</f>
+        <v>5</v>
+      </c>
+      <c r="O28">
+        <f>MIN(K28:K37)</f>
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29">
+        <v>0.999</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
+        <v>0.999</v>
+      </c>
+      <c r="M29" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29">
+        <f>AVERAGE(J28:J37)</f>
+        <v>6.3</v>
+      </c>
+      <c r="O29">
+        <f>AVERAGE(K28:K37)</f>
+        <v>0.99130000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30">
+        <v>0.98</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
+      </c>
+      <c r="K30">
+        <v>0.98</v>
+      </c>
+      <c r="M30" t="s">
+        <v>36</v>
+      </c>
+      <c r="N30">
+        <f>MAX(J28:J37)</f>
+        <v>9</v>
+      </c>
+      <c r="O30">
+        <f>MAX(K28:K37)</f>
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31">
+        <v>0.996</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33">
+        <v>0.999</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="K33">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35">
+        <v>0.997</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37">
+        <v>0.996</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="M40" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40">
+        <f>MIN(J40:J49)</f>
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <f>MIN(K40:K49)</f>
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41">
+        <v>0.998</v>
+      </c>
+      <c r="J41">
+        <v>7</v>
+      </c>
+      <c r="K41">
+        <v>0.998</v>
+      </c>
+      <c r="M41" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41">
+        <f>AVERAGE(J40:J49)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O41">
+        <f>AVERAGE(K40:K49)</f>
+        <v>0.9929</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="K42">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="M42" t="s">
+        <v>36</v>
+      </c>
+      <c r="N42">
+        <f>MAX(J40:J49)</f>
+        <v>7</v>
+      </c>
+      <c r="O42">
+        <f>MAX(K40:K49)</f>
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43">
+        <v>0.996</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+      <c r="K44">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45">
+        <v>0.999</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+      <c r="K45">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46">
+        <v>0.995</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48">
+        <v>6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J48">
+        <v>6</v>
+      </c>
+      <c r="K48">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>0.99099999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53">
+        <v>0.99</v>
+      </c>
+      <c r="J53">
+        <v>10</v>
+      </c>
+      <c r="K53">
+        <v>0.99</v>
+      </c>
+      <c r="M53" t="s">
+        <v>32</v>
+      </c>
+      <c r="N53">
+        <f>MIN(J53:J62)</f>
+        <v>9</v>
+      </c>
+      <c r="O53">
+        <f>MIN(K53:K62)</f>
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="J54">
+        <v>13</v>
+      </c>
+      <c r="K54">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="M54" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54">
+        <f>AVERAGE(J53:J62)</f>
+        <v>10.9</v>
+      </c>
+      <c r="O54">
+        <f>AVERAGE(K53:K62)</f>
+        <v>0.9778</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J55">
+        <v>12</v>
+      </c>
+      <c r="K55">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="M55" t="s">
+        <v>36</v>
+      </c>
+      <c r="N55">
+        <f>MAX(J53:J62)</f>
+        <v>13</v>
+      </c>
+      <c r="O55">
+        <f>MAX(K53:K62)</f>
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="J56">
+        <v>12</v>
+      </c>
+      <c r="K56">
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="J57">
+        <v>11</v>
+      </c>
+      <c r="K57">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58">
+        <v>0.996</v>
+      </c>
+      <c r="J58">
+        <v>11</v>
+      </c>
+      <c r="K58">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+      <c r="G59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="J59">
+        <v>10</v>
+      </c>
+      <c r="K59">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60">
+        <v>9</v>
+      </c>
+      <c r="G60" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="J60">
+        <v>9</v>
+      </c>
+      <c r="K60">
+        <v>0.96399999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J61">
+        <v>12</v>
+      </c>
+      <c r="K61">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62">
+        <v>9</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J62">
+        <v>9</v>
+      </c>
+      <c r="K62">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="J65">
+        <v>9</v>
+      </c>
+      <c r="K65">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="M65" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65">
+        <f>MIN(J65:J74)</f>
+        <v>8</v>
+      </c>
+      <c r="O65">
+        <f>MIN(K65:K74)</f>
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66">
+        <v>13</v>
+      </c>
+      <c r="G66" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J66">
+        <v>13</v>
+      </c>
+      <c r="K66">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="M66" t="s">
+        <v>34</v>
+      </c>
+      <c r="N66">
+        <f>AVERAGE(J65:J74)</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O66">
+        <f>AVERAGE(K65:K74)</f>
+        <v>0.97359999999999991</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="J67">
+        <v>11</v>
+      </c>
+      <c r="K67">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="M67" t="s">
+        <v>36</v>
+      </c>
+      <c r="N67">
+        <f>MAX(J65:J74)</f>
+        <v>13</v>
+      </c>
+      <c r="O67">
+        <f>MAX(K65:K74)</f>
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" t="s">
+        <v>23</v>
+      </c>
+      <c r="F68">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="J68">
+        <v>12</v>
+      </c>
+      <c r="K68">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" t="s">
+        <v>23</v>
+      </c>
+      <c r="F69">
+        <v>10</v>
+      </c>
+      <c r="G69" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="J69">
+        <v>10</v>
+      </c>
+      <c r="K69">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" t="s">
+        <v>23</v>
+      </c>
+      <c r="F70">
+        <v>10</v>
+      </c>
+      <c r="G70" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="J70">
+        <v>10</v>
+      </c>
+      <c r="K70">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="J71">
+        <v>9</v>
+      </c>
+      <c r="K71">
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="J72">
+        <v>9</v>
+      </c>
+      <c r="K72">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="J73">
+        <v>11</v>
+      </c>
+      <c r="K73">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74">
+        <v>8</v>
+      </c>
+      <c r="G74" t="s">
+        <v>24</v>
+      </c>
+      <c r="H74">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J74">
+        <v>8</v>
+      </c>
+      <c r="K74">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77">
+        <v>9</v>
+      </c>
+      <c r="G77" t="s">
+        <v>24</v>
+      </c>
+      <c r="H77">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="J77">
+        <v>9</v>
+      </c>
+      <c r="K77">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="M77" t="s">
+        <v>32</v>
+      </c>
+      <c r="N77">
+        <f>MIN(J77:J86)</f>
+        <v>8</v>
+      </c>
+      <c r="O77">
+        <f>MIN(K77:K86)</f>
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78">
+        <v>13</v>
+      </c>
+      <c r="G78" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J78">
+        <v>13</v>
+      </c>
+      <c r="K78">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="M78" t="s">
+        <v>34</v>
+      </c>
+      <c r="N78">
+        <f>AVERAGE(J77:J86)</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O78">
+        <f>AVERAGE(K77:K86)</f>
+        <v>0.97299999999999986</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="J79">
+        <v>11</v>
+      </c>
+      <c r="K79">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="M79" t="s">
+        <v>36</v>
+      </c>
+      <c r="N79">
+        <f>MAX(J77:J86)</f>
+        <v>13</v>
+      </c>
+      <c r="O79">
+        <f>MAX(K77:K86)</f>
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" t="s">
+        <v>23</v>
+      </c>
+      <c r="F80">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="J80">
+        <v>12</v>
+      </c>
+      <c r="K80">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="J81">
+        <v>10</v>
+      </c>
+      <c r="K81">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" t="s">
+        <v>23</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J82">
+        <v>10</v>
+      </c>
+      <c r="K82">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83">
+        <v>9</v>
+      </c>
+      <c r="G83" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="J83">
+        <v>9</v>
+      </c>
+      <c r="K83">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84">
+        <v>9</v>
+      </c>
+      <c r="G84" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="J84">
+        <v>9</v>
+      </c>
+      <c r="K84">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85">
+        <v>11</v>
+      </c>
+      <c r="G85" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="J85">
+        <v>11</v>
+      </c>
+      <c r="K85">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" t="s">
+        <v>23</v>
+      </c>
+      <c r="F86">
+        <v>8</v>
+      </c>
+      <c r="G86" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J86">
+        <v>8</v>
+      </c>
+      <c r="K86">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89">
+        <v>8</v>
+      </c>
+      <c r="G89" t="s">
+        <v>24</v>
+      </c>
+      <c r="H89">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J89">
+        <v>8</v>
+      </c>
+      <c r="K89">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="M89" t="s">
+        <v>32</v>
+      </c>
+      <c r="N89">
+        <f>MIN(J89:J98)</f>
+        <v>7</v>
+      </c>
+      <c r="O89">
+        <f>MIN(K89:K98)</f>
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>22</v>
+      </c>
+      <c r="E90" t="s">
+        <v>23</v>
+      </c>
+      <c r="F90">
+        <v>11</v>
+      </c>
+      <c r="G90" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="J90">
+        <v>11</v>
+      </c>
+      <c r="K90">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="M90" t="s">
+        <v>34</v>
+      </c>
+      <c r="N90">
+        <f>AVERAGE(J89:J98)</f>
+        <v>8.9</v>
+      </c>
+      <c r="O90">
+        <f>AVERAGE(K89:K98)</f>
+        <v>0.97929999999999995</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91">
+        <v>10</v>
+      </c>
+      <c r="G91" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J91">
+        <v>10</v>
+      </c>
+      <c r="K91">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="M91" t="s">
+        <v>36</v>
+      </c>
+      <c r="N91">
+        <f>MAX(J89:J98)</f>
+        <v>11</v>
+      </c>
+      <c r="O91">
+        <f>MAX(K89:K98)</f>
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
+        <v>23</v>
+      </c>
+      <c r="F92">
+        <v>11</v>
+      </c>
+      <c r="G92" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92">
+        <v>0.999</v>
+      </c>
+      <c r="J92">
+        <v>11</v>
+      </c>
+      <c r="K92">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" t="s">
+        <v>23</v>
+      </c>
+      <c r="F93">
+        <v>9</v>
+      </c>
+      <c r="G93" t="s">
+        <v>24</v>
+      </c>
+      <c r="H93">
+        <v>0.99</v>
+      </c>
+      <c r="J93">
+        <v>9</v>
+      </c>
+      <c r="K93">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94" t="s">
+        <v>23</v>
+      </c>
+      <c r="F94">
+        <v>8</v>
+      </c>
+      <c r="G94" t="s">
+        <v>24</v>
+      </c>
+      <c r="H94">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="J94">
+        <v>8</v>
+      </c>
+      <c r="K94">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
+        <v>21</v>
+      </c>
+      <c r="C95">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" t="s">
+        <v>23</v>
+      </c>
+      <c r="F95">
+        <v>8</v>
+      </c>
+      <c r="G95" t="s">
+        <v>24</v>
+      </c>
+      <c r="H95">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="J95">
+        <v>8</v>
+      </c>
+      <c r="K95">
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>20</v>
+      </c>
+      <c r="B96" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" t="s">
+        <v>23</v>
+      </c>
+      <c r="F96">
+        <v>7</v>
+      </c>
+      <c r="G96" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="J96">
+        <v>7</v>
+      </c>
+      <c r="K96">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" t="s">
+        <v>21</v>
+      </c>
+      <c r="C97">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97">
+        <v>10</v>
+      </c>
+      <c r="G97" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="J97">
+        <v>10</v>
+      </c>
+      <c r="K97">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" t="s">
+        <v>21</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98" t="s">
+        <v>22</v>
+      </c>
+      <c r="E98" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98">
+        <v>7</v>
+      </c>
+      <c r="G98" t="s">
+        <v>24</v>
+      </c>
+      <c r="H98">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J98">
+        <v>7</v>
+      </c>
+      <c r="K98">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" t="s">
+        <v>23</v>
+      </c>
+      <c r="F101">
+        <v>7</v>
+      </c>
+      <c r="G101" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J101">
+        <v>7</v>
+      </c>
+      <c r="K101">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="M101" t="s">
+        <v>32</v>
+      </c>
+      <c r="N101">
+        <f>MIN(J101:J110)</f>
+        <v>6</v>
+      </c>
+      <c r="O101">
+        <f>MIN(K101:K110)</f>
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" t="s">
+        <v>23</v>
+      </c>
+      <c r="F102">
+        <v>10</v>
+      </c>
+      <c r="G102" t="s">
+        <v>24</v>
+      </c>
+      <c r="H102">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="J102">
+        <v>10</v>
+      </c>
+      <c r="K102">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="M102" t="s">
+        <v>34</v>
+      </c>
+      <c r="N102">
+        <f>AVERAGE(J101:J110)</f>
+        <v>7.8</v>
+      </c>
+      <c r="O102">
+        <f>AVERAGE(K101:K110)</f>
+        <v>0.98029999999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>22</v>
+      </c>
+      <c r="E103" t="s">
+        <v>23</v>
+      </c>
+      <c r="F103">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J103">
+        <v>9</v>
+      </c>
+      <c r="K103">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="M103" t="s">
+        <v>36</v>
+      </c>
+      <c r="N103">
+        <f>MAX(J101:J110)</f>
+        <v>10</v>
+      </c>
+      <c r="O103">
+        <f>MAX(K101:K110)</f>
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>21</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>22</v>
+      </c>
+      <c r="E104" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104">
+        <v>9</v>
+      </c>
+      <c r="G104" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J104">
+        <v>9</v>
+      </c>
+      <c r="K104">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s">
+        <v>21</v>
+      </c>
+      <c r="C105">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" t="s">
+        <v>23</v>
+      </c>
+      <c r="F105">
+        <v>8</v>
+      </c>
+      <c r="G105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H105">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J105">
+        <v>8</v>
+      </c>
+      <c r="K105">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
+      </c>
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>23</v>
+      </c>
+      <c r="F106">
+        <v>7</v>
+      </c>
+      <c r="G106" t="s">
+        <v>24</v>
+      </c>
+      <c r="H106">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J106">
+        <v>7</v>
+      </c>
+      <c r="K106">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>21</v>
+      </c>
+      <c r="C107">
+        <v>7</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
+      </c>
+      <c r="E107" t="s">
+        <v>23</v>
+      </c>
+      <c r="F107">
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
+        <v>24</v>
+      </c>
+      <c r="H107">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="J107">
+        <v>7</v>
+      </c>
+      <c r="K107">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108">
+        <v>8</v>
+      </c>
+      <c r="D108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" t="s">
+        <v>23</v>
+      </c>
+      <c r="F108">
+        <v>6</v>
+      </c>
+      <c r="G108" t="s">
+        <v>24</v>
+      </c>
+      <c r="H108">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="J108">
+        <v>6</v>
+      </c>
+      <c r="K108">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>20</v>
+      </c>
+      <c r="B109" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" t="s">
+        <v>23</v>
+      </c>
+      <c r="F109">
+        <v>9</v>
+      </c>
+      <c r="G109" t="s">
+        <v>24</v>
+      </c>
+      <c r="H109">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J109">
+        <v>9</v>
+      </c>
+      <c r="K109">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110">
+        <v>10</v>
+      </c>
+      <c r="D110" t="s">
+        <v>22</v>
+      </c>
+      <c r="E110" t="s">
+        <v>23</v>
+      </c>
+      <c r="F110">
+        <v>6</v>
+      </c>
+      <c r="G110" t="s">
+        <v>24</v>
+      </c>
+      <c r="H110">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="J110">
+        <v>6</v>
+      </c>
+      <c r="K110">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="117" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="U117" s="1"/>
+      <c r="V117" s="1"/>
+      <c r="W117" s="1"/>
+      <c r="X117" s="1"/>
+      <c r="Y117" s="1"/>
+      <c r="Z117" s="1"/>
+      <c r="AA117" s="1"/>
+      <c r="AB117" s="1"/>
+      <c r="AC117" s="1"/>
+      <c r="AD117" s="1"/>
+      <c r="AE117" s="1"/>
+      <c r="AF117" s="1"/>
+      <c r="AG117" s="1"/>
+      <c r="AH117" s="1"/>
+    </row>
+    <row r="118" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="U118" s="1"/>
+      <c r="V118" s="1"/>
+      <c r="W118" s="1"/>
+      <c r="X118" s="1"/>
+      <c r="Y118" s="1"/>
+      <c r="Z118" s="1"/>
+      <c r="AA118" s="1"/>
+      <c r="AB118" s="1"/>
+      <c r="AC118" s="1"/>
+      <c r="AD118" s="1"/>
+      <c r="AE118" s="1"/>
+      <c r="AF118" s="1"/>
+      <c r="AG118" s="1"/>
+      <c r="AH118" s="1"/>
+    </row>
+    <row r="119" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="U119" s="1"/>
+      <c r="V119" s="1"/>
+      <c r="W119" s="1"/>
+      <c r="X119" s="1"/>
+      <c r="Y119" s="1"/>
+      <c r="Z119" s="1"/>
+      <c r="AA119" s="1"/>
+      <c r="AB119" s="1"/>
+      <c r="AC119" s="1"/>
+      <c r="AD119" s="1"/>
+      <c r="AE119" s="1"/>
+      <c r="AF119" s="1"/>
+      <c r="AG119" s="1"/>
+      <c r="AH119" s="1"/>
+    </row>
+    <row r="124" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="G124" s="2"/>
+      <c r="H124" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L124" s="3"/>
+      <c r="M124" s="3"/>
+    </row>
+    <row r="125" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="G125" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="G126" s="2">
         <v>0.1</v>
       </c>
-      <c r="C11">
+      <c r="H126" s="2">
+        <v>6</v>
+      </c>
+      <c r="I126" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="J126" s="2">
+        <v>11</v>
+      </c>
+      <c r="K126" s="2">
+        <v>9</v>
+      </c>
+      <c r="L126" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="M126" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="G127" s="2">
         <v>0.13</v>
       </c>
-      <c r="D11">
+      <c r="H127" s="2">
+        <v>6</v>
+      </c>
+      <c r="I127" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="J127" s="2">
+        <v>10</v>
+      </c>
+      <c r="K127" s="2">
+        <v>8</v>
+      </c>
+      <c r="L127" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M127" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="7:34" x14ac:dyDescent="0.2">
+      <c r="G128" s="2">
         <v>0.16</v>
       </c>
-      <c r="E11">
+      <c r="H128" s="2">
+        <v>5</v>
+      </c>
+      <c r="I128" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="J128" s="2">
+        <v>9</v>
+      </c>
+      <c r="K128" s="2">
+        <v>8</v>
+      </c>
+      <c r="L128" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M128" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="G129" s="2">
         <v>0.19</v>
       </c>
-      <c r="F11">
+      <c r="H129" s="2">
+        <v>3</v>
+      </c>
+      <c r="I129" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J129" s="2">
+        <v>7</v>
+      </c>
+      <c r="K129" s="2">
+        <v>7</v>
+      </c>
+      <c r="L129" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="M129" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="G130" s="2">
         <v>0.22</v>
       </c>
-      <c r="G11">
-        <v>0.25</v>
-      </c>
-      <c r="H11">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I11">
-        <v>0.31</v>
-      </c>
-      <c r="J11">
-        <v>0.34</v>
-      </c>
-      <c r="K11">
-        <v>0.37</v>
-      </c>
-      <c r="L11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <f>1-B8</f>
-        <v>0.22860000000000003</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:F12" si="0">1-C8</f>
-        <v>0.20369999999999999</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.20420000000000005</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0.15100000000000002</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.11730000000000007</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0.1</v>
-      </c>
-      <c r="B15">
-        <v>209</v>
-      </c>
-      <c r="C15">
-        <v>232</v>
-      </c>
-      <c r="D15">
-        <v>63</v>
-      </c>
-      <c r="E15">
-        <v>178</v>
-      </c>
-      <c r="F15">
-        <v>247</v>
-      </c>
-      <c r="G15">
-        <v>18</v>
-      </c>
-      <c r="H15">
-        <v>210</v>
-      </c>
-      <c r="I15">
-        <v>235</v>
-      </c>
-      <c r="J15">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>0.13</v>
-      </c>
-      <c r="B16">
-        <v>161</v>
-      </c>
-      <c r="C16">
-        <v>237</v>
-      </c>
-      <c r="D16">
+      <c r="H130" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K130" s="2">
+        <v>6</v>
+      </c>
+      <c r="L130" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="M130" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
+        <v>31</v>
+      </c>
+      <c r="D137">
+        <v>6</v>
+      </c>
+      <c r="E137">
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C138" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138">
+        <v>8.4</v>
+      </c>
+      <c r="E138">
+        <v>0.98580000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C139" t="s">
+        <v>35</v>
+      </c>
+      <c r="D139">
+        <v>11</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
+        <v>31</v>
+      </c>
+      <c r="D149">
+        <v>6</v>
+      </c>
+      <c r="E149">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="150" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C150" t="s">
+        <v>33</v>
+      </c>
+      <c r="D150">
+        <v>7.3</v>
+      </c>
+      <c r="E150">
+        <v>0.98629999999999995</v>
+      </c>
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C151" t="s">
+        <v>35</v>
+      </c>
+      <c r="D151">
+        <v>10</v>
+      </c>
+      <c r="E151">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="161" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
+        <v>31</v>
+      </c>
+      <c r="D161">
+        <v>5</v>
+      </c>
+      <c r="E161">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C162" t="s">
+        <v>33</v>
+      </c>
+      <c r="D162">
+        <v>6.3</v>
+      </c>
+      <c r="E162">
+        <v>0.99130000000000007</v>
+      </c>
+    </row>
+    <row r="163" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C163" t="s">
+        <v>35</v>
+      </c>
+      <c r="D163">
+        <v>9</v>
+      </c>
+      <c r="E163">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="173" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
+        <v>31</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="174" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C174" t="s">
+        <v>33</v>
+      </c>
+      <c r="D174">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E174">
+        <v>0.9929</v>
+      </c>
+    </row>
+    <row r="175" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C175" t="s">
+        <v>35</v>
+      </c>
+      <c r="D175">
+        <v>7</v>
+      </c>
+      <c r="E175">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C186" t="s">
+        <v>31</v>
+      </c>
+      <c r="D186">
+        <v>9</v>
+      </c>
+      <c r="E186">
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="187" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C187" t="s">
+        <v>33</v>
+      </c>
+      <c r="D187">
+        <v>10.9</v>
+      </c>
+      <c r="E187">
+        <v>0.9778</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C188" t="s">
+        <v>35</v>
+      </c>
+      <c r="D188">
         <v>13</v>
       </c>
-      <c r="E16">
-        <v>231</v>
-      </c>
-      <c r="F16">
-        <v>240</v>
-      </c>
-      <c r="G16">
-        <v>61</v>
-      </c>
-      <c r="H16">
-        <v>196</v>
-      </c>
-      <c r="I16">
-        <v>222</v>
-      </c>
-      <c r="J16">
+      <c r="E188">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="198" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C198" t="s">
+        <v>31</v>
+      </c>
+      <c r="D198">
+        <v>8</v>
+      </c>
+      <c r="E198">
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="199" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
+        <v>33</v>
+      </c>
+      <c r="D199">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E199">
+        <v>0.97359999999999991</v>
+      </c>
+    </row>
+    <row r="200" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
+        <v>35</v>
+      </c>
+      <c r="D200">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0.16</v>
-      </c>
-      <c r="B17">
-        <v>157</v>
-      </c>
-      <c r="C17">
-        <v>240</v>
-      </c>
-      <c r="D17">
+      <c r="E200">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
+        <v>31</v>
+      </c>
+      <c r="D210">
+        <v>8</v>
+      </c>
+      <c r="E210">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="211" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
+        <v>33</v>
+      </c>
+      <c r="D211">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E211">
+        <v>0.97299999999999986</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C212" t="s">
+        <v>35</v>
+      </c>
+      <c r="D212">
         <v>13</v>
       </c>
-      <c r="E17">
-        <v>215</v>
-      </c>
-      <c r="F17">
-        <v>249</v>
-      </c>
-      <c r="G17">
-        <v>39</v>
-      </c>
-      <c r="H17">
-        <v>180</v>
-      </c>
-      <c r="I17">
-        <v>250</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0.19</v>
-      </c>
-      <c r="B18">
-        <v>175</v>
-      </c>
-      <c r="C18">
-        <v>236</v>
-      </c>
-      <c r="D18">
-        <v>14</v>
-      </c>
-      <c r="E18">
-        <v>234</v>
-      </c>
-      <c r="F18">
-        <v>244</v>
-      </c>
-      <c r="G18">
-        <v>52</v>
-      </c>
-      <c r="H18">
-        <v>201</v>
-      </c>
-      <c r="I18">
-        <v>244</v>
-      </c>
-      <c r="J18">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0.22</v>
-      </c>
-      <c r="B19">
-        <v>199</v>
-      </c>
-      <c r="C19">
-        <v>249</v>
-      </c>
-      <c r="D19">
-        <v>51</v>
-      </c>
-      <c r="E19">
-        <v>205</v>
-      </c>
-      <c r="F19">
-        <v>238</v>
-      </c>
-      <c r="G19">
-        <v>55</v>
-      </c>
-      <c r="H19">
-        <v>201</v>
-      </c>
-      <c r="I19">
-        <v>241</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
+      <c r="E212">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="222" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C222" t="s">
+        <v>31</v>
+      </c>
+      <c r="D222">
+        <v>7</v>
+      </c>
+      <c r="E222">
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="223" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C223" t="s">
+        <v>33</v>
+      </c>
+      <c r="D223">
+        <v>8.9</v>
+      </c>
+      <c r="E223">
+        <v>0.97929999999999995</v>
+      </c>
+    </row>
+    <row r="224" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C224" t="s">
+        <v>35</v>
+      </c>
+      <c r="D224">
+        <v>11</v>
+      </c>
+      <c r="E224">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="234" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C234" t="s">
+        <v>31</v>
+      </c>
+      <c r="D234">
+        <v>6</v>
+      </c>
+      <c r="E234">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="235" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C235" t="s">
+        <v>33</v>
+      </c>
+      <c r="D235">
+        <v>7.8</v>
+      </c>
+      <c r="E235">
+        <v>0.98029999999999995</v>
+      </c>
+    </row>
+    <row r="236" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C236" t="s">
+        <v>35</v>
+      </c>
+      <c r="D236">
+        <v>10</v>
+      </c>
+      <c r="E236">
+        <v>0.99299999999999999</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="U117:AA119"/>
+    <mergeCell ref="AB117:AH119"/>
+    <mergeCell ref="H124:J124"/>
+    <mergeCell ref="K124:M124"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEF222D-36D1-4B8E-8345-D42416BA344B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF994A4-4F16-49F7-801D-0743ACE2881D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -739,7 +4329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933EA071-E3DF-40AF-9890-4575FDD17572}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -753,6 +4343,272 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE1F27B-438F-49BB-B1F9-9E2E3BFD9632}">
+  <dimension ref="A8:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0.77139999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.79630000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.79579999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="F8">
+        <f>0.6627+0.22</f>
+        <v>0.88269999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+      <c r="C11">
+        <v>0.13</v>
+      </c>
+      <c r="D11">
+        <v>0.16</v>
+      </c>
+      <c r="E11">
+        <v>0.19</v>
+      </c>
+      <c r="F11">
+        <v>0.22</v>
+      </c>
+      <c r="G11">
+        <v>0.25</v>
+      </c>
+      <c r="H11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I11">
+        <v>0.31</v>
+      </c>
+      <c r="J11">
+        <v>0.34</v>
+      </c>
+      <c r="K11">
+        <v>0.37</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f>1-B8</f>
+        <v>0.22860000000000003</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:F12" si="0">1-C8</f>
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.20420000000000005</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.11730000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.1</v>
+      </c>
+      <c r="B15">
+        <v>209</v>
+      </c>
+      <c r="C15">
+        <v>232</v>
+      </c>
+      <c r="D15">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>178</v>
+      </c>
+      <c r="F15">
+        <v>247</v>
+      </c>
+      <c r="G15">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>210</v>
+      </c>
+      <c r="I15">
+        <v>235</v>
+      </c>
+      <c r="J15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.13</v>
+      </c>
+      <c r="B16">
+        <v>161</v>
+      </c>
+      <c r="C16">
+        <v>237</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>231</v>
+      </c>
+      <c r="F16">
+        <v>240</v>
+      </c>
+      <c r="G16">
+        <v>61</v>
+      </c>
+      <c r="H16">
+        <v>196</v>
+      </c>
+      <c r="I16">
+        <v>222</v>
+      </c>
+      <c r="J16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.16</v>
+      </c>
+      <c r="B17">
+        <v>157</v>
+      </c>
+      <c r="C17">
+        <v>240</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>215</v>
+      </c>
+      <c r="F17">
+        <v>249</v>
+      </c>
+      <c r="G17">
+        <v>39</v>
+      </c>
+      <c r="H17">
+        <v>180</v>
+      </c>
+      <c r="I17">
+        <v>250</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.19</v>
+      </c>
+      <c r="B18">
+        <v>175</v>
+      </c>
+      <c r="C18">
+        <v>236</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>234</v>
+      </c>
+      <c r="F18">
+        <v>244</v>
+      </c>
+      <c r="G18">
+        <v>52</v>
+      </c>
+      <c r="H18">
+        <v>201</v>
+      </c>
+      <c r="I18">
+        <v>244</v>
+      </c>
+      <c r="J18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.22</v>
+      </c>
+      <c r="B19">
+        <v>199</v>
+      </c>
+      <c r="C19">
+        <v>249</v>
+      </c>
+      <c r="D19">
+        <v>51</v>
+      </c>
+      <c r="E19">
+        <v>205</v>
+      </c>
+      <c r="F19">
+        <v>238</v>
+      </c>
+      <c r="G19">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>201</v>
+      </c>
+      <c r="I19">
+        <v>241</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CB0D64-59B8-459C-A01E-8E4AA2A4B171}">
   <dimension ref="A1:J113"/>
   <sheetViews>
@@ -2632,7 +6488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA540F61-8CF0-4232-8E10-DFA7CB778057}">
   <dimension ref="A1:J113"/>
   <sheetViews>
@@ -4512,7 +8368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F784F1-4FF5-4B7A-912B-E81DF9CE5DCC}">
   <dimension ref="A1:J119"/>
   <sheetViews>
@@ -6402,7 +10258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A860ACA-9657-412A-ACC2-3B1B824919E9}">
   <dimension ref="A2:J119"/>
   <sheetViews>
@@ -8290,7 +12146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111F5B06-8EF8-4861-88C7-096B22705BFE}">
   <dimension ref="A1:N116"/>
   <sheetViews>
@@ -10180,7 +14036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24476271-F492-4731-AD77-13EBDC110CF0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10193,7 +14049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6637A8-60E8-42CD-BA1D-6610345C7913}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10204,17 +14060,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEF222D-36D1-4B8E-8345-D42416BA344B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
results updated in E3 table
</commit_message>
<xml_diff>
--- a/result/E3.xlsx
+++ b/result/E3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhaos\Desktop\research-dual-period\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA65EF6-1194-42FF-8FB7-DD4CC709A8F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E84562-1C8D-458E-8133-330B4C114D31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C7D420CA-42D4-4E62-9CB7-56532C9F3227}"/>
+    <workbookView xWindow="12540" yWindow="3765" windowWidth="23550" windowHeight="12945" activeTab="1" xr2:uid="{C7D420CA-42D4-4E62-9CB7-56532C9F3227}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="45">
   <si>
     <t>Best</t>
   </si>
@@ -181,11 +181,26 @@
     <t>U</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>single</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,9 +240,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -235,8 +253,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE8625D-1816-4CE6-97F4-E7BD14C709EC}">
   <dimension ref="A1:AH236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="P135" sqref="P135"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124:M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3796,55 +3814,55 @@
       </c>
     </row>
     <row r="117" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="U117" s="1"/>
-      <c r="V117" s="1"/>
-      <c r="W117" s="1"/>
-      <c r="X117" s="1"/>
-      <c r="Y117" s="1"/>
-      <c r="Z117" s="1"/>
-      <c r="AA117" s="1"/>
-      <c r="AB117" s="1"/>
-      <c r="AC117" s="1"/>
-      <c r="AD117" s="1"/>
-      <c r="AE117" s="1"/>
-      <c r="AF117" s="1"/>
-      <c r="AG117" s="1"/>
-      <c r="AH117" s="1"/>
+      <c r="U117" s="2"/>
+      <c r="V117" s="2"/>
+      <c r="W117" s="2"/>
+      <c r="X117" s="2"/>
+      <c r="Y117" s="2"/>
+      <c r="Z117" s="2"/>
+      <c r="AA117" s="2"/>
+      <c r="AB117" s="2"/>
+      <c r="AC117" s="2"/>
+      <c r="AD117" s="2"/>
+      <c r="AE117" s="2"/>
+      <c r="AF117" s="2"/>
+      <c r="AG117" s="2"/>
+      <c r="AH117" s="2"/>
     </row>
     <row r="118" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="U118" s="1"/>
-      <c r="V118" s="1"/>
-      <c r="W118" s="1"/>
-      <c r="X118" s="1"/>
-      <c r="Y118" s="1"/>
-      <c r="Z118" s="1"/>
-      <c r="AA118" s="1"/>
-      <c r="AB118" s="1"/>
-      <c r="AC118" s="1"/>
-      <c r="AD118" s="1"/>
-      <c r="AE118" s="1"/>
-      <c r="AF118" s="1"/>
-      <c r="AG118" s="1"/>
-      <c r="AH118" s="1"/>
+      <c r="U118" s="2"/>
+      <c r="V118" s="2"/>
+      <c r="W118" s="2"/>
+      <c r="X118" s="2"/>
+      <c r="Y118" s="2"/>
+      <c r="Z118" s="2"/>
+      <c r="AA118" s="2"/>
+      <c r="AB118" s="2"/>
+      <c r="AC118" s="2"/>
+      <c r="AD118" s="2"/>
+      <c r="AE118" s="2"/>
+      <c r="AF118" s="2"/>
+      <c r="AG118" s="2"/>
+      <c r="AH118" s="2"/>
     </row>
     <row r="119" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="U119" s="1"/>
-      <c r="V119" s="1"/>
-      <c r="W119" s="1"/>
-      <c r="X119" s="1"/>
-      <c r="Y119" s="1"/>
-      <c r="Z119" s="1"/>
-      <c r="AA119" s="1"/>
-      <c r="AB119" s="1"/>
-      <c r="AC119" s="1"/>
-      <c r="AD119" s="1"/>
-      <c r="AE119" s="1"/>
-      <c r="AF119" s="1"/>
-      <c r="AG119" s="1"/>
-      <c r="AH119" s="1"/>
+      <c r="U119" s="2"/>
+      <c r="V119" s="2"/>
+      <c r="W119" s="2"/>
+      <c r="X119" s="2"/>
+      <c r="Y119" s="2"/>
+      <c r="Z119" s="2"/>
+      <c r="AA119" s="2"/>
+      <c r="AB119" s="2"/>
+      <c r="AC119" s="2"/>
+      <c r="AD119" s="2"/>
+      <c r="AE119" s="2"/>
+      <c r="AF119" s="2"/>
+      <c r="AG119" s="2"/>
+      <c r="AH119" s="2"/>
     </row>
     <row r="124" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="G124" s="2"/>
+      <c r="G124" s="1"/>
       <c r="H124" s="3" t="s">
         <v>37</v>
       </c>
@@ -3857,140 +3875,140 @@
       <c r="M124" s="3"/>
     </row>
     <row r="125" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="G125" s="2" t="s">
+      <c r="G125" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="H125" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I125" s="2" t="s">
+      <c r="I125" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="J125" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K125" s="2" t="s">
+      <c r="K125" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="L125" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M125" s="2" t="s">
+      <c r="M125" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="126" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="G126" s="2">
+      <c r="G126" s="1">
         <v>0.1</v>
       </c>
-      <c r="H126" s="2">
+      <c r="H126" s="1">
         <v>6</v>
       </c>
-      <c r="I126" s="2">
+      <c r="I126" s="1">
         <v>8.4</v>
       </c>
-      <c r="J126" s="2">
+      <c r="J126" s="1">
         <v>11</v>
       </c>
-      <c r="K126" s="2">
+      <c r="K126" s="1">
         <v>9</v>
       </c>
-      <c r="L126" s="2">
+      <c r="L126" s="1">
         <v>10.9</v>
       </c>
-      <c r="M126" s="2">
+      <c r="M126" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="127" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="G127" s="2">
+      <c r="G127" s="1">
         <v>0.13</v>
       </c>
-      <c r="H127" s="2">
+      <c r="H127" s="1">
         <v>6</v>
       </c>
-      <c r="I127" s="2">
+      <c r="I127" s="1">
         <v>7.3</v>
       </c>
-      <c r="J127" s="2">
+      <c r="J127" s="1">
         <v>10</v>
       </c>
-      <c r="K127" s="2">
+      <c r="K127" s="1">
         <v>8</v>
       </c>
-      <c r="L127" s="2">
+      <c r="L127" s="1">
         <v>10.199999999999999</v>
       </c>
-      <c r="M127" s="2">
+      <c r="M127" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="128" spans="7:34" x14ac:dyDescent="0.2">
-      <c r="G128" s="2">
+      <c r="G128" s="1">
         <v>0.16</v>
       </c>
-      <c r="H128" s="2">
+      <c r="H128" s="1">
         <v>5</v>
       </c>
-      <c r="I128" s="2">
+      <c r="I128" s="1">
         <v>6.3</v>
       </c>
-      <c r="J128" s="2">
+      <c r="J128" s="1">
         <v>9</v>
       </c>
-      <c r="K128" s="2">
+      <c r="K128" s="1">
         <v>8</v>
       </c>
-      <c r="L128" s="2">
+      <c r="L128" s="1">
         <v>10.199999999999999</v>
       </c>
-      <c r="M128" s="2">
+      <c r="M128" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="129" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="G129" s="2">
+      <c r="G129" s="1">
         <v>0.19</v>
       </c>
-      <c r="H129" s="2">
+      <c r="H129" s="1">
         <v>3</v>
       </c>
-      <c r="I129" s="2">
+      <c r="I129" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J129" s="2">
+      <c r="J129" s="1">
         <v>7</v>
       </c>
-      <c r="K129" s="2">
+      <c r="K129" s="1">
         <v>7</v>
       </c>
-      <c r="L129" s="2">
+      <c r="L129" s="1">
         <v>8.9</v>
       </c>
-      <c r="M129" s="2">
+      <c r="M129" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="130" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="G130" s="2">
+      <c r="G130" s="1">
         <v>0.22</v>
       </c>
-      <c r="H130" s="2" t="s">
+      <c r="H130" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I130" s="2" t="s">
+      <c r="I130" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J130" s="2" t="s">
+      <c r="J130" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K130" s="2">
+      <c r="K130" s="1">
         <v>6</v>
       </c>
-      <c r="L130" s="2">
+      <c r="L130" s="1">
         <v>7.8</v>
       </c>
-      <c r="M130" s="2">
+      <c r="M130" s="1">
         <v>10</v>
       </c>
     </row>
@@ -4344,10 +4362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE1F27B-438F-49BB-B1F9-9E2E3BFD9632}">
-  <dimension ref="A8:L19"/>
+  <dimension ref="A8:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4505,7 +4523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.16</v>
       </c>
@@ -4537,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.19</v>
       </c>
@@ -4569,7 +4587,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.22</v>
       </c>
@@ -4598,6 +4616,102 @@
         <v>241</v>
       </c>
       <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>0.1</v>
+      </c>
+      <c r="F24">
+        <v>0.13</v>
+      </c>
+      <c r="G24">
+        <v>0.16</v>
+      </c>
+      <c r="H24">
+        <v>0.19</v>
+      </c>
+      <c r="I24">
+        <v>0.22</v>
+      </c>
+      <c r="J24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="F25" s="4">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="H25" s="4">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.2286</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.20420000000000005</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.11730000000000007</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="4">
+        <f>E26-E25</f>
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" ref="F27:J27" si="1">F26-F25</f>
+        <v>0.1051</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13560000000000005</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11240000000000003</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11730000000000007</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>